<commit_message>
further data exploration with IIHS
</commit_message>
<xml_diff>
--- a/Resources/Condition of U.S. Roadways by Functional System.xlsx
+++ b/Resources/Condition of U.S. Roadways by Functional System.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\NTS\2018\Q1\Federal Review\To Web Team\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7fc1888e1acd26e6/Documents/GIT/Project1/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A3F88577-30EE-45DA-8526-9DC24EA6433B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="3900" windowWidth="15480" windowHeight="5310" tabRatio="975"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11950" tabRatio="975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-27" sheetId="1" r:id="rId1"/>
@@ -43,7 +44,7 @@
     <definedName name="SHEET3">#REF!</definedName>
     <definedName name="SHEET4">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -204,14 +205,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="###0.00_)"/>
     <numFmt numFmtId="165" formatCode="#,##0_)"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -592,29 +593,11 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -623,51 +606,97 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="34">
-    <cellStyle name="Data" xfId="1"/>
-    <cellStyle name="Data no deci" xfId="2"/>
-    <cellStyle name="Data Superscript" xfId="3"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="4"/>
-    <cellStyle name="Hed Side" xfId="5"/>
-    <cellStyle name="Hed Side bold" xfId="6"/>
-    <cellStyle name="Hed Side Indent" xfId="7"/>
-    <cellStyle name="Hed Side Regular" xfId="8"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="9"/>
-    <cellStyle name="Hed Top" xfId="10"/>
+    <cellStyle name="Data" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Data no deci" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Data Superscript" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Hed Side" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Hed Side bold" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Hed Side Indent" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Hed Side Regular" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Hed Top" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="11"/>
-    <cellStyle name="Normal 3" xfId="12"/>
-    <cellStyle name="Normal 4" xfId="13"/>
-    <cellStyle name="Normal 5" xfId="14"/>
-    <cellStyle name="Normal 6" xfId="33"/>
-    <cellStyle name="Source Hed" xfId="15"/>
-    <cellStyle name="Source Superscript" xfId="16"/>
-    <cellStyle name="Source Text" xfId="17"/>
-    <cellStyle name="State" xfId="18"/>
-    <cellStyle name="Superscript" xfId="19"/>
-    <cellStyle name="Table Data" xfId="20"/>
-    <cellStyle name="Table Head Top" xfId="21"/>
-    <cellStyle name="Table Hed Side" xfId="22"/>
-    <cellStyle name="Table Title" xfId="23"/>
-    <cellStyle name="Title Text" xfId="24"/>
-    <cellStyle name="Title Text 1" xfId="25"/>
-    <cellStyle name="Title Text 2" xfId="26"/>
-    <cellStyle name="Title-1" xfId="27"/>
-    <cellStyle name="Title-2" xfId="28"/>
-    <cellStyle name="Title-3" xfId="29"/>
-    <cellStyle name="Wrap" xfId="30"/>
-    <cellStyle name="Wrap Bold" xfId="31"/>
-    <cellStyle name="Wrap Title" xfId="32"/>
+    <cellStyle name="Normal 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 3" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 4" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 5" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 6" xfId="33" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Source Hed" xfId="15" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Source Superscript" xfId="16" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Source Text" xfId="17" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="State" xfId="18" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Superscript" xfId="19" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Table Data" xfId="20" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Table Head Top" xfId="21" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Table Hed Side" xfId="22" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Table Title" xfId="23" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Title Text" xfId="24" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Title Text 1" xfId="25" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Title Text 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Title-1" xfId="27" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Title-2" xfId="28" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Title-3" xfId="29" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Wrap" xfId="30" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Wrap Bold" xfId="31" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Wrap Title" xfId="32" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{691DD2BC-A727-435B-987C-8907294E3411}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -999,7 +1028,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1009,46 +1038,46 @@
       <selection sqref="A1:Z1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="1" customWidth="1"/>
-    <col min="2" max="19" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.453125" style="1" customWidth="1"/>
+    <col min="2" max="19" width="7.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="26" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="1"/>
+    <col min="21" max="26" width="7.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:26" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-    </row>
-    <row r="2" spans="1:26" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+    </row>
+    <row r="2" spans="1:26" s="7" customFormat="1" ht="16.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -1128,7 +1157,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1145,7 +1174,7 @@
       <c r="L3" s="11"/>
       <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -1225,7 +1254,7 @@
         <v>28818.797000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>20</v>
       </c>
@@ -1305,7 +1334,7 @@
         <v>0.51454958373175641</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A6" s="16" t="s">
         <v>21</v>
       </c>
@@ -1385,7 +1414,7 @@
         <v>1.4564036104629901</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>22</v>
       </c>
@@ -1465,7 +1494,7 @@
         <v>14.475396040993664</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>23</v>
       </c>
@@ -1545,7 +1574,7 @@
         <v>33.992504961258447</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>24</v>
       </c>
@@ -1625,7 +1654,7 @@
         <v>49.561145803553138</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
@@ -1705,7 +1734,7 @@
         <v>314.45999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A11" s="21" t="s">
         <v>4</v>
       </c>
@@ -1785,7 +1814,7 @@
         <v>86113.032000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>20</v>
       </c>
@@ -1865,7 +1894,7 @@
         <v>1.3582218310464318</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>21</v>
       </c>
@@ -1945,7 +1974,7 @@
         <v>3.0018069738852073</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>22</v>
       </c>
@@ -2025,7 +2054,7 @@
         <v>26.796480699924714</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>23</v>
       </c>
@@ -2105,7 +2134,7 @@
         <v>41.11614023763557</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A16" s="16" t="s">
         <v>24</v>
       </c>
@@ -2185,7 +2214,7 @@
         <v>27.727350257508053</v>
       </c>
     </row>
-    <row r="17" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
@@ -2265,7 +2294,7 @@
         <v>3614.806</v>
       </c>
     </row>
-    <row r="18" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A18" s="21" t="s">
         <v>5</v>
       </c>
@@ -2345,7 +2374,7 @@
         <v>112786.29276000001</v>
       </c>
     </row>
-    <row r="19" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>20</v>
       </c>
@@ -2425,7 +2454,7 @@
         <v>2.4713255767092028</v>
       </c>
     </row>
-    <row r="20" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A20" s="16" t="s">
         <v>21</v>
       </c>
@@ -2505,7 +2534,7 @@
         <v>5.5332486841107524</v>
       </c>
     </row>
-    <row r="21" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A21" s="16" t="s">
         <v>22</v>
       </c>
@@ -2585,7 +2614,7 @@
         <v>37.334514930464842</v>
       </c>
     </row>
-    <row r="22" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A22" s="16" t="s">
         <v>23</v>
       </c>
@@ -2665,7 +2694,7 @@
         <v>39.480365246823801</v>
       </c>
     </row>
-    <row r="23" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A23" s="16" t="s">
         <v>24</v>
       </c>
@@ -2745,7 +2774,7 @@
         <v>15.180545561891387</v>
       </c>
     </row>
-    <row r="24" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A24" s="8" t="s">
         <v>15</v>
       </c>
@@ -2825,7 +2854,7 @@
         <v>1426.7773799999998</v>
       </c>
     </row>
-    <row r="25" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A25" s="21" t="s">
         <v>6</v>
       </c>
@@ -2905,7 +2934,7 @@
         <v>233129.77413999996</v>
       </c>
     </row>
-    <row r="26" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A26" s="16" t="s">
         <v>20</v>
       </c>
@@ -2985,7 +3014,7 @@
         <v>10.223756621360062</v>
       </c>
     </row>
-    <row r="27" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A27" s="16" t="s">
         <v>21</v>
       </c>
@@ -3065,7 +3094,7 @@
         <v>11.731247585551319</v>
       </c>
     </row>
-    <row r="28" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A28" s="16" t="s">
         <v>22</v>
       </c>
@@ -3145,7 +3174,7 @@
         <v>44.216559364955593</v>
       </c>
     </row>
-    <row r="29" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A29" s="16" t="s">
         <v>23</v>
       </c>
@@ -3225,7 +3254,7 @@
         <v>27.036885396778349</v>
       </c>
     </row>
-    <row r="30" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A30" s="16" t="s">
         <v>24</v>
       </c>
@@ -3305,7 +3334,7 @@
         <v>6.7915510313546781</v>
       </c>
     </row>
-    <row r="31" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A31" s="8" t="s">
         <v>15</v>
       </c>
@@ -3385,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A32" s="8"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -3413,7 +3442,7 @@
       <c r="Y32" s="20"/>
       <c r="Z32" s="20"/>
     </row>
-    <row r="33" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1">
       <c r="A33" s="8" t="s">
         <v>10</v>
       </c>
@@ -3443,7 +3472,7 @@
       <c r="Y33" s="20"/>
       <c r="Z33" s="20"/>
     </row>
-    <row r="34" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A34" s="8" t="s">
         <v>3</v>
       </c>
@@ -3523,7 +3552,7 @@
         <v>18514.753999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A35" s="16" t="s">
         <v>20</v>
       </c>
@@ -3603,7 +3632,7 @@
         <v>1.5623215949831144</v>
       </c>
     </row>
-    <row r="36" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A36" s="16" t="s">
         <v>21</v>
       </c>
@@ -3683,7 +3712,7 @@
         <v>3.6648069966255026</v>
       </c>
     </row>
-    <row r="37" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A37" s="16" t="s">
         <v>22</v>
       </c>
@@ -3763,7 +3792,7 @@
         <v>23.564968781113706</v>
       </c>
     </row>
-    <row r="38" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A38" s="16" t="s">
         <v>23</v>
       </c>
@@ -3843,7 +3872,7 @@
         <v>35.36233319654152</v>
       </c>
     </row>
-    <row r="39" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A39" s="16" t="s">
         <v>24</v>
       </c>
@@ -3923,7 +3952,7 @@
         <v>35.845569430736148</v>
       </c>
     </row>
-    <row r="40" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A40" s="8" t="s">
         <v>15</v>
       </c>
@@ -4003,7 +4032,7 @@
         <v>543.74199999999996</v>
       </c>
     </row>
-    <row r="41" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A41" s="21" t="s">
         <v>7</v>
       </c>
@@ -4083,7 +4112,7 @@
         <v>11632.759000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A42" s="16" t="s">
         <v>20</v>
       </c>
@@ -4163,7 +4192,7 @@
         <v>2.8384409923733482</v>
       </c>
     </row>
-    <row r="43" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A43" s="16" t="s">
         <v>21</v>
       </c>
@@ -4243,7 +4272,7 @@
         <v>5.6479378623764145</v>
       </c>
     </row>
-    <row r="44" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A44" s="16" t="s">
         <v>22</v>
       </c>
@@ -4323,7 +4352,7 @@
         <v>31.741696015536807</v>
       </c>
     </row>
-    <row r="45" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A45" s="16" t="s">
         <v>23</v>
       </c>
@@ -4403,7 +4432,7 @@
         <v>37.385043393403052</v>
       </c>
     </row>
-    <row r="46" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A46" s="16" t="s">
         <v>24</v>
       </c>
@@ -4483,7 +4512,7 @@
         <v>22.386881736310361</v>
       </c>
     </row>
-    <row r="47" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A47" s="8" t="s">
         <v>15</v>
       </c>
@@ -4563,7 +4592,7 @@
         <v>621.84599999999989</v>
       </c>
     </row>
-    <row r="48" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A48" s="21" t="s">
         <v>4</v>
       </c>
@@ -4643,7 +4672,7 @@
         <v>62466.727000000021</v>
       </c>
     </row>
-    <row r="49" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A49" s="16" t="s">
         <v>20</v>
       </c>
@@ -4723,7 +4752,7 @@
         <v>14.069955994332789</v>
       </c>
     </row>
-    <row r="50" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A50" s="16" t="s">
         <v>21</v>
       </c>
@@ -4803,7 +4832,7 @@
         <v>12.720419944525021</v>
       </c>
     </row>
-    <row r="51" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A51" s="16" t="s">
         <v>22</v>
       </c>
@@ -4883,7 +4912,7 @@
         <v>38.909568609221338</v>
       </c>
     </row>
-    <row r="52" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A52" s="16" t="s">
         <v>23</v>
       </c>
@@ -4963,7 +4992,7 @@
         <v>24.421913445216987</v>
       </c>
     </row>
-    <row r="53" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A53" s="16" t="s">
         <v>24</v>
       </c>
@@ -5043,7 +5072,7 @@
         <v>9.8781420067038219</v>
       </c>
     </row>
-    <row r="54" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A54" s="8" t="s">
         <v>15</v>
       </c>
@@ -5123,7 +5152,7 @@
         <v>3670.4769999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A55" s="21" t="s">
         <v>5</v>
       </c>
@@ -5203,7 +5232,7 @@
         <v>71938.274200000014</v>
       </c>
     </row>
-    <row r="56" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A56" s="16" t="s">
         <v>20</v>
       </c>
@@ -5283,7 +5312,7 @@
         <v>19.111927291689184</v>
       </c>
     </row>
-    <row r="57" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A57" s="16" t="s">
         <v>21</v>
       </c>
@@ -5363,7 +5392,7 @@
         <v>16.98348422431296</v>
       </c>
     </row>
-    <row r="58" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A58" s="16" t="s">
         <v>22</v>
       </c>
@@ -5443,7 +5472,7 @@
         <v>42.400362754323616</v>
       </c>
     </row>
-    <row r="59" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A59" s="16" t="s">
         <v>23</v>
       </c>
@@ -5523,7 +5552,7 @@
         <v>17.506645412408297</v>
       </c>
     </row>
-    <row r="60" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A60" s="16" t="s">
         <v>24</v>
       </c>
@@ -5603,7 +5632,7 @@
         <v>3.9975803172659363</v>
       </c>
     </row>
-    <row r="61" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A61" s="8" t="s">
         <v>15</v>
       </c>
@@ -5683,7 +5712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A62" s="8" t="s">
         <v>8</v>
       </c>
@@ -5763,7 +5792,7 @@
         <v>82662.935500000021</v>
       </c>
     </row>
-    <row r="63" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A63" s="16" t="s">
         <v>20</v>
       </c>
@@ -5843,7 +5872,7 @@
         <v>30.503025325056349</v>
       </c>
     </row>
-    <row r="64" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A64" s="16" t="s">
         <v>21</v>
       </c>
@@ -5923,7 +5952,7 @@
         <v>20.28326979750193</v>
       </c>
     </row>
-    <row r="65" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A65" s="16" t="s">
         <v>22</v>
       </c>
@@ -6003,7 +6032,7 @@
         <v>37.501254247134732</v>
       </c>
     </row>
-    <row r="66" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A66" s="16" t="s">
         <v>23</v>
       </c>
@@ -6083,7 +6112,7 @@
         <v>10.435156721478878</v>
       </c>
     </row>
-    <row r="67" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1">
       <c r="A67" s="16" t="s">
         <v>24</v>
       </c>
@@ -6163,7 +6192,7 @@
         <v>1.2772939088280988</v>
       </c>
     </row>
-    <row r="68" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:26" s="20" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
       <c r="A68" s="8" t="s">
         <v>15</v>
       </c>
@@ -6243,185 +6272,185 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:26" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="32" t="s">
+    <row r="69" spans="1:26" s="32" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A69" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B69" s="32"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="32"/>
-      <c r="E69" s="32"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="32"/>
-      <c r="H69" s="32"/>
-      <c r="I69" s="32"/>
-      <c r="J69" s="32"/>
-      <c r="K69" s="32"/>
-      <c r="L69" s="32"/>
-      <c r="M69" s="32"/>
-      <c r="N69" s="32"/>
-      <c r="O69" s="32"/>
-      <c r="P69" s="32"/>
-      <c r="Q69" s="32"/>
-      <c r="R69" s="32"/>
-      <c r="S69" s="32"/>
-      <c r="T69" s="32"/>
-      <c r="U69" s="32"/>
-      <c r="V69" s="32"/>
-      <c r="W69" s="32"/>
-      <c r="X69" s="32"/>
-      <c r="Y69" s="32"/>
-      <c r="Z69" s="32"/>
-    </row>
-    <row r="70" spans="1:26" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="34"/>
-      <c r="B70" s="34"/>
-      <c r="C70" s="34"/>
-      <c r="D70" s="34"/>
-      <c r="E70" s="34"/>
-      <c r="F70" s="34"/>
-      <c r="G70" s="34"/>
-      <c r="H70" s="34"/>
-      <c r="I70" s="34"/>
-      <c r="J70" s="34"/>
-      <c r="K70" s="34"/>
-      <c r="L70" s="34"/>
-      <c r="M70" s="34"/>
-      <c r="N70" s="34"/>
-      <c r="O70" s="34"/>
-      <c r="P70" s="34"/>
-      <c r="Q70" s="34"/>
-      <c r="R70" s="34"/>
-      <c r="S70" s="34"/>
-      <c r="T70" s="34"/>
-      <c r="U70" s="34"/>
-      <c r="V70" s="34"/>
-      <c r="W70" s="34"/>
-      <c r="X70" s="34"/>
-      <c r="Y70" s="34"/>
-      <c r="Z70" s="34"/>
-    </row>
-    <row r="71" spans="1:26" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="35" t="s">
+      <c r="B69" s="42"/>
+      <c r="C69" s="42"/>
+      <c r="D69" s="42"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="42"/>
+      <c r="H69" s="42"/>
+      <c r="I69" s="42"/>
+      <c r="J69" s="42"/>
+      <c r="K69" s="42"/>
+      <c r="L69" s="42"/>
+      <c r="M69" s="42"/>
+      <c r="N69" s="42"/>
+      <c r="O69" s="42"/>
+      <c r="P69" s="42"/>
+      <c r="Q69" s="42"/>
+      <c r="R69" s="42"/>
+      <c r="S69" s="42"/>
+      <c r="T69" s="42"/>
+      <c r="U69" s="42"/>
+      <c r="V69" s="42"/>
+      <c r="W69" s="42"/>
+      <c r="X69" s="42"/>
+      <c r="Y69" s="42"/>
+      <c r="Z69" s="42"/>
+    </row>
+    <row r="70" spans="1:26" s="32" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A70" s="43"/>
+      <c r="B70" s="43"/>
+      <c r="C70" s="43"/>
+      <c r="D70" s="43"/>
+      <c r="E70" s="43"/>
+      <c r="F70" s="43"/>
+      <c r="G70" s="43"/>
+      <c r="H70" s="43"/>
+      <c r="I70" s="43"/>
+      <c r="J70" s="43"/>
+      <c r="K70" s="43"/>
+      <c r="L70" s="43"/>
+      <c r="M70" s="43"/>
+      <c r="N70" s="43"/>
+      <c r="O70" s="43"/>
+      <c r="P70" s="43"/>
+      <c r="Q70" s="43"/>
+      <c r="R70" s="43"/>
+      <c r="S70" s="43"/>
+      <c r="T70" s="43"/>
+      <c r="U70" s="43"/>
+      <c r="V70" s="43"/>
+      <c r="W70" s="43"/>
+      <c r="X70" s="43"/>
+      <c r="Y70" s="43"/>
+      <c r="Z70" s="43"/>
+    </row>
+    <row r="71" spans="1:26" s="32" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A71" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B71" s="35"/>
-      <c r="C71" s="35"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="35"/>
-      <c r="G71" s="35"/>
-      <c r="H71" s="35"/>
-      <c r="I71" s="35"/>
-      <c r="J71" s="35"/>
-      <c r="K71" s="35"/>
-      <c r="L71" s="35"/>
-      <c r="M71" s="35"/>
-      <c r="N71" s="35"/>
-      <c r="O71" s="35"/>
-      <c r="P71" s="35"/>
-      <c r="Q71" s="35"/>
-      <c r="R71" s="35"/>
-      <c r="S71" s="35"/>
-      <c r="T71" s="35"/>
-      <c r="U71" s="35"/>
-      <c r="V71" s="35"/>
-      <c r="W71" s="35"/>
-      <c r="X71" s="35"/>
-      <c r="Y71" s="35"/>
-      <c r="Z71" s="35"/>
-    </row>
-    <row r="72" spans="1:26" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="36" t="s">
+      <c r="B71" s="44"/>
+      <c r="C71" s="44"/>
+      <c r="D71" s="44"/>
+      <c r="E71" s="44"/>
+      <c r="F71" s="44"/>
+      <c r="G71" s="44"/>
+      <c r="H71" s="44"/>
+      <c r="I71" s="44"/>
+      <c r="J71" s="44"/>
+      <c r="K71" s="44"/>
+      <c r="L71" s="44"/>
+      <c r="M71" s="44"/>
+      <c r="N71" s="44"/>
+      <c r="O71" s="44"/>
+      <c r="P71" s="44"/>
+      <c r="Q71" s="44"/>
+      <c r="R71" s="44"/>
+      <c r="S71" s="44"/>
+      <c r="T71" s="44"/>
+      <c r="U71" s="44"/>
+      <c r="V71" s="44"/>
+      <c r="W71" s="44"/>
+      <c r="X71" s="44"/>
+      <c r="Y71" s="44"/>
+      <c r="Z71" s="44"/>
+    </row>
+    <row r="72" spans="1:26" s="32" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A72" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B72" s="36"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
-      <c r="G72" s="36"/>
-      <c r="H72" s="36"/>
-      <c r="I72" s="36"/>
-      <c r="J72" s="36"/>
-      <c r="K72" s="36"/>
-      <c r="L72" s="36"/>
-      <c r="M72" s="36"/>
-      <c r="N72" s="36"/>
-      <c r="O72" s="36"/>
-      <c r="P72" s="36"/>
-      <c r="Q72" s="36"/>
-      <c r="R72" s="36"/>
-      <c r="S72" s="36"/>
-      <c r="T72" s="36"/>
-      <c r="U72" s="36"/>
-      <c r="V72" s="36"/>
-      <c r="W72" s="36"/>
-      <c r="X72" s="36"/>
-      <c r="Y72" s="36"/>
-      <c r="Z72" s="36"/>
-    </row>
-    <row r="73" spans="1:26" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="36" t="s">
+      <c r="B72" s="37"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="37"/>
+      <c r="G72" s="37"/>
+      <c r="H72" s="37"/>
+      <c r="I72" s="37"/>
+      <c r="J72" s="37"/>
+      <c r="K72" s="37"/>
+      <c r="L72" s="37"/>
+      <c r="M72" s="37"/>
+      <c r="N72" s="37"/>
+      <c r="O72" s="37"/>
+      <c r="P72" s="37"/>
+      <c r="Q72" s="37"/>
+      <c r="R72" s="37"/>
+      <c r="S72" s="37"/>
+      <c r="T72" s="37"/>
+      <c r="U72" s="37"/>
+      <c r="V72" s="37"/>
+      <c r="W72" s="37"/>
+      <c r="X72" s="37"/>
+      <c r="Y72" s="37"/>
+      <c r="Z72" s="37"/>
+    </row>
+    <row r="73" spans="1:26" s="32" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A73" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B73" s="36"/>
-      <c r="C73" s="36"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="36"/>
-      <c r="G73" s="36"/>
-      <c r="H73" s="36"/>
-      <c r="I73" s="36"/>
-      <c r="J73" s="36"/>
-      <c r="K73" s="36"/>
-      <c r="L73" s="36"/>
-      <c r="M73" s="36"/>
-      <c r="N73" s="36"/>
-      <c r="O73" s="36"/>
-      <c r="P73" s="36"/>
-      <c r="Q73" s="36"/>
-      <c r="R73" s="36"/>
-      <c r="S73" s="36"/>
-      <c r="T73" s="36"/>
-      <c r="U73" s="36"/>
-      <c r="V73" s="36"/>
-      <c r="W73" s="36"/>
-      <c r="X73" s="36"/>
-      <c r="Y73" s="36"/>
-      <c r="Z73" s="36"/>
-    </row>
-    <row r="74" spans="1:26" s="38" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="37" t="s">
+      <c r="B73" s="37"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="37"/>
+      <c r="F73" s="37"/>
+      <c r="G73" s="37"/>
+      <c r="H73" s="37"/>
+      <c r="I73" s="37"/>
+      <c r="J73" s="37"/>
+      <c r="K73" s="37"/>
+      <c r="L73" s="37"/>
+      <c r="M73" s="37"/>
+      <c r="N73" s="37"/>
+      <c r="O73" s="37"/>
+      <c r="P73" s="37"/>
+      <c r="Q73" s="37"/>
+      <c r="R73" s="37"/>
+      <c r="S73" s="37"/>
+      <c r="T73" s="37"/>
+      <c r="U73" s="37"/>
+      <c r="V73" s="37"/>
+      <c r="W73" s="37"/>
+      <c r="X73" s="37"/>
+      <c r="Y73" s="37"/>
+      <c r="Z73" s="37"/>
+    </row>
+    <row r="74" spans="1:26" s="33" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A74" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B74" s="37"/>
-      <c r="C74" s="37"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="37"/>
-      <c r="G74" s="37"/>
-      <c r="H74" s="37"/>
-      <c r="I74" s="37"/>
-      <c r="J74" s="37"/>
-      <c r="K74" s="37"/>
-      <c r="L74" s="37"/>
-      <c r="M74" s="37"/>
-      <c r="N74" s="37"/>
-      <c r="O74" s="37"/>
-      <c r="P74" s="37"/>
-      <c r="Q74" s="37"/>
-      <c r="R74" s="37"/>
-      <c r="S74" s="37"/>
-      <c r="T74" s="37"/>
-      <c r="U74" s="37"/>
-      <c r="V74" s="37"/>
-      <c r="W74" s="37"/>
-      <c r="X74" s="37"/>
-      <c r="Y74" s="37"/>
-      <c r="Z74" s="37"/>
-    </row>
-    <row r="75" spans="1:26" s="38" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="38"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="38"/>
+      <c r="H74" s="38"/>
+      <c r="I74" s="38"/>
+      <c r="J74" s="38"/>
+      <c r="K74" s="38"/>
+      <c r="L74" s="38"/>
+      <c r="M74" s="38"/>
+      <c r="N74" s="38"/>
+      <c r="O74" s="38"/>
+      <c r="P74" s="38"/>
+      <c r="Q74" s="38"/>
+      <c r="R74" s="38"/>
+      <c r="S74" s="38"/>
+      <c r="T74" s="38"/>
+      <c r="U74" s="38"/>
+      <c r="V74" s="38"/>
+      <c r="W74" s="38"/>
+      <c r="X74" s="38"/>
+      <c r="Y74" s="38"/>
+      <c r="Z74" s="38"/>
+    </row>
+    <row r="75" spans="1:26" s="33" customFormat="1" ht="12.75" customHeight="1">
       <c r="A75" s="39"/>
       <c r="B75" s="39"/>
       <c r="C75" s="39"/>
@@ -6449,7 +6478,7 @@
       <c r="Y75" s="39"/>
       <c r="Z75" s="39"/>
     </row>
-    <row r="76" spans="1:26" s="38" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" s="33" customFormat="1" ht="12.75" customHeight="1">
       <c r="A76" s="40" t="s">
         <v>1</v>
       </c>
@@ -6479,128 +6508,132 @@
       <c r="Y76" s="40"/>
       <c r="Z76" s="40"/>
     </row>
-    <row r="77" spans="1:26" s="38" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="41" t="s">
+    <row r="77" spans="1:26" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A77" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B77" s="41"/>
-      <c r="C77" s="41"/>
-      <c r="D77" s="41"/>
-      <c r="E77" s="41"/>
-      <c r="F77" s="41"/>
-      <c r="G77" s="41"/>
-      <c r="H77" s="41"/>
-      <c r="I77" s="41"/>
-      <c r="J77" s="41"/>
-      <c r="K77" s="41"/>
-      <c r="L77" s="41"/>
-      <c r="M77" s="41"/>
-      <c r="N77" s="41"/>
-      <c r="O77" s="41"/>
-      <c r="P77" s="41"/>
-      <c r="Q77" s="41"/>
-      <c r="R77" s="41"/>
-      <c r="S77" s="41"/>
-      <c r="T77" s="41"/>
-      <c r="U77" s="41"/>
-      <c r="V77" s="41"/>
-      <c r="W77" s="41"/>
-      <c r="X77" s="41"/>
-      <c r="Y77" s="41"/>
-      <c r="Z77" s="41"/>
-    </row>
-    <row r="78" spans="1:26" s="43" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="42" t="s">
+      <c r="B77" s="35"/>
+      <c r="C77" s="35"/>
+      <c r="D77" s="35"/>
+      <c r="E77" s="35"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="35"/>
+      <c r="H77" s="35"/>
+      <c r="I77" s="35"/>
+      <c r="J77" s="35"/>
+      <c r="K77" s="35"/>
+      <c r="L77" s="35"/>
+      <c r="M77" s="35"/>
+      <c r="N77" s="35"/>
+      <c r="O77" s="35"/>
+      <c r="P77" s="35"/>
+      <c r="Q77" s="35"/>
+      <c r="R77" s="35"/>
+      <c r="S77" s="35"/>
+      <c r="T77" s="35"/>
+      <c r="U77" s="35"/>
+      <c r="V77" s="35"/>
+      <c r="W77" s="35"/>
+      <c r="X77" s="35"/>
+      <c r="Y77" s="35"/>
+      <c r="Z77" s="35"/>
+    </row>
+    <row r="78" spans="1:26" s="34" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A78" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B78" s="42"/>
-      <c r="C78" s="42"/>
-      <c r="D78" s="42"/>
-      <c r="E78" s="42"/>
-      <c r="F78" s="42"/>
-      <c r="G78" s="42"/>
-      <c r="H78" s="42"/>
-      <c r="I78" s="42"/>
-      <c r="J78" s="42"/>
-      <c r="K78" s="42"/>
-      <c r="L78" s="42"/>
-      <c r="M78" s="42"/>
-      <c r="N78" s="42"/>
-      <c r="O78" s="42"/>
-      <c r="P78" s="42"/>
-      <c r="Q78" s="42"/>
-      <c r="R78" s="42"/>
-      <c r="S78" s="42"/>
-      <c r="T78" s="42"/>
-      <c r="U78" s="42"/>
-      <c r="V78" s="42"/>
-      <c r="W78" s="42"/>
-      <c r="X78" s="42"/>
-      <c r="Y78" s="42"/>
-      <c r="Z78" s="42"/>
-    </row>
-    <row r="79" spans="1:26" s="38" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="41" t="s">
+      <c r="B78" s="36"/>
+      <c r="C78" s="36"/>
+      <c r="D78" s="36"/>
+      <c r="E78" s="36"/>
+      <c r="F78" s="36"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="36"/>
+      <c r="I78" s="36"/>
+      <c r="J78" s="36"/>
+      <c r="K78" s="36"/>
+      <c r="L78" s="36"/>
+      <c r="M78" s="36"/>
+      <c r="N78" s="36"/>
+      <c r="O78" s="36"/>
+      <c r="P78" s="36"/>
+      <c r="Q78" s="36"/>
+      <c r="R78" s="36"/>
+      <c r="S78" s="36"/>
+      <c r="T78" s="36"/>
+      <c r="U78" s="36"/>
+      <c r="V78" s="36"/>
+      <c r="W78" s="36"/>
+      <c r="X78" s="36"/>
+      <c r="Y78" s="36"/>
+      <c r="Z78" s="36"/>
+    </row>
+    <row r="79" spans="1:26" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A79" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B79" s="41"/>
-      <c r="C79" s="41"/>
-      <c r="D79" s="41"/>
-      <c r="E79" s="41"/>
-      <c r="F79" s="41"/>
-      <c r="G79" s="41"/>
-      <c r="H79" s="41"/>
-      <c r="I79" s="41"/>
-      <c r="J79" s="41"/>
-      <c r="K79" s="41"/>
-      <c r="L79" s="41"/>
-      <c r="M79" s="41"/>
-      <c r="N79" s="41"/>
-      <c r="O79" s="41"/>
-      <c r="P79" s="41"/>
-      <c r="Q79" s="41"/>
-      <c r="R79" s="41"/>
-      <c r="S79" s="41"/>
-      <c r="T79" s="41"/>
-      <c r="U79" s="41"/>
-      <c r="V79" s="41"/>
-      <c r="W79" s="41"/>
-      <c r="X79" s="41"/>
-      <c r="Y79" s="41"/>
-      <c r="Z79" s="41"/>
-    </row>
-    <row r="80" spans="1:26" s="38" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="42" t="s">
+      <c r="B79" s="35"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="35"/>
+      <c r="E79" s="35"/>
+      <c r="F79" s="35"/>
+      <c r="G79" s="35"/>
+      <c r="H79" s="35"/>
+      <c r="I79" s="35"/>
+      <c r="J79" s="35"/>
+      <c r="K79" s="35"/>
+      <c r="L79" s="35"/>
+      <c r="M79" s="35"/>
+      <c r="N79" s="35"/>
+      <c r="O79" s="35"/>
+      <c r="P79" s="35"/>
+      <c r="Q79" s="35"/>
+      <c r="R79" s="35"/>
+      <c r="S79" s="35"/>
+      <c r="T79" s="35"/>
+      <c r="U79" s="35"/>
+      <c r="V79" s="35"/>
+      <c r="W79" s="35"/>
+      <c r="X79" s="35"/>
+      <c r="Y79" s="35"/>
+      <c r="Z79" s="35"/>
+    </row>
+    <row r="80" spans="1:26" s="33" customFormat="1" ht="12" customHeight="1">
+      <c r="A80" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B80" s="42"/>
-      <c r="C80" s="42"/>
-      <c r="D80" s="42"/>
-      <c r="E80" s="42"/>
-      <c r="F80" s="42"/>
-      <c r="G80" s="42"/>
-      <c r="H80" s="42"/>
-      <c r="I80" s="42"/>
-      <c r="J80" s="42"/>
-      <c r="K80" s="42"/>
-      <c r="L80" s="42"/>
-      <c r="M80" s="42"/>
-      <c r="N80" s="42"/>
-      <c r="O80" s="42"/>
-      <c r="P80" s="42"/>
-      <c r="Q80" s="42"/>
-      <c r="R80" s="42"/>
-      <c r="S80" s="42"/>
-      <c r="T80" s="42"/>
-      <c r="U80" s="42"/>
-      <c r="V80" s="42"/>
-      <c r="W80" s="42"/>
-      <c r="X80" s="42"/>
-      <c r="Y80" s="42"/>
-      <c r="Z80" s="42"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="36"/>
+      <c r="D80" s="36"/>
+      <c r="E80" s="36"/>
+      <c r="F80" s="36"/>
+      <c r="G80" s="36"/>
+      <c r="H80" s="36"/>
+      <c r="I80" s="36"/>
+      <c r="J80" s="36"/>
+      <c r="K80" s="36"/>
+      <c r="L80" s="36"/>
+      <c r="M80" s="36"/>
+      <c r="N80" s="36"/>
+      <c r="O80" s="36"/>
+      <c r="P80" s="36"/>
+      <c r="Q80" s="36"/>
+      <c r="R80" s="36"/>
+      <c r="S80" s="36"/>
+      <c r="T80" s="36"/>
+      <c r="U80" s="36"/>
+      <c r="V80" s="36"/>
+      <c r="W80" s="36"/>
+      <c r="X80" s="36"/>
+      <c r="Y80" s="36"/>
+      <c r="Z80" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:Z1"/>
+    <mergeCell ref="A69:Z69"/>
+    <mergeCell ref="A70:Z70"/>
+    <mergeCell ref="A71:Z71"/>
     <mergeCell ref="A77:Z77"/>
     <mergeCell ref="A78:Z78"/>
     <mergeCell ref="A79:Z79"/>
@@ -6610,10 +6643,6 @@
     <mergeCell ref="A74:Z74"/>
     <mergeCell ref="A75:Z75"/>
     <mergeCell ref="A76:Z76"/>
-    <mergeCell ref="A1:Z1"/>
-    <mergeCell ref="A69:Z69"/>
-    <mergeCell ref="A70:Z70"/>
-    <mergeCell ref="A71:Z71"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6623,6 +6652,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002817D3A329724A479313C886C2FB1746" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="62a8723b96c1432a91a35108219c4d81">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e9378d88-8176-4f71-9851-64a93c091a10" xmlns:ns3="b7325b2c-accd-4278-8079-34cb29d0c829" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a07d12f4bfae53195ebfca05177dd56" ns2:_="" ns3:_="">
     <xsd:import namespace="e9378d88-8176-4f71-9851-64a93c091a10"/>
@@ -6787,29 +6831,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44EB4903-2884-438F-9B60-584527CB2D19}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF77D1C3-4926-43F1-AE77-0B8A47532563}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{215DF15D-BA9F-4CFB-A5BF-7D34462FDF30}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{215DF15D-BA9F-4CFB-A5BF-7D34462FDF30}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF77D1C3-4926-43F1-AE77-0B8A47532563}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44EB4903-2884-438F-9B60-584527CB2D19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e9378d88-8176-4f71-9851-64a93c091a10"/>
+    <ds:schemaRef ds:uri="b7325b2c-accd-4278-8079-34cb29d0c829"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>